<commit_message>
Atualização em janela index e no texto
</commit_message>
<xml_diff>
--- a/API_semestre1_pythonators-main/Janelas/data_base/Pasta1.xlsx
+++ b/API_semestre1_pythonators-main/Janelas/data_base/Pasta1.xlsx
@@ -450,19 +450,19 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>